<commit_message>
Bill_Rate patterns added with fallback extractor
</commit_message>
<xml_diff>
--- a/Active 20260120 - Copy.xlsx
+++ b/Active 20260120 - Copy.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\OneDrive\Documents\Beeline JD Parser\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c5e77caf6b479126/Documents/Beeline JD Parser/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49132ED0-984B-4905-BBD2-F197B89F9026}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="13_ncr:1_{49132ED0-984B-4905-BBD2-F197B89F9026}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5E475747-C7AD-4F86-8680-92EC3026CD3B}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="24">
   <si>
     <t>Job Code</t>
   </si>
@@ -98,12 +98,33 @@
   <si>
     <t>Description</t>
   </si>
+  <si>
+    <t xml:space="preserve">            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">                </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Job Description: **Please strictly adhere to the following resume naming convention:ALL CAPS, NO SPACES B/T UNDERSCORESMax Bill Rate: $95/hrPTN_US_GBAMSREQID_CandidateBeelineIDi.e. PTN_US_9999999_SKIPJOHNSON0413MSP Owner: Deepa NarayananLocation: San Jose CADuration: 6 monthsGBaMS ReqID: 10441358 100% Onsite. *** LOCAL CANDIDATES ONLY***Developer - Go, Python, JavaJob Requirements:• 4-5+ years production level experience with distributed applications at scale in public and/or private cloud• Experience architecting and implementing large scale Observability platforms• B.S. degree in Computer Science or related technical field• Work in a diverse and distributed team environment!Must Have• Programming experience with languages like Go, Python, Java; Experience building integrations and applications to large-scale environments. • Experience with UI technologies like JavaScript, React, backstage etc.• Experience with internally hosted Observability and Tooling systems like Splunk, Prometheus, GitHub, Jenkins, Artifactory, assisting clients and improving environment performance and stability• Experience with container platforms like Kubernetes• Experience designing and implementing systems for fault tolerance, scalability and stability.• Experience developing, deploying and running distributed applications on cloud platforms. Experience with container and orchestration technologies (Docker, Kubernetes)• Ensure the highest level of up-time and Quality of Service (QoS) to Adobe’s customers through operational excellence• Knowledge in defining service level objectives (SLOs) and service level indicators (SLIs) to represent and measure service quality• Knowledge of (public and/or private) cloud• Collaborate with SRE and Engineering/Product teams in driving critical initiatives.• Experience in solving performance and stability issues using a wide variety of tools• Exceptional communicator in and across teams, driving projects to completion• Impacts the organization through contribution to technical direction and strategic decisions.Additional Sills: 
+						 Skills:
+										Category
+										Name
+										Required
+										Importance
+										Experience
+                    SkillCategoryTest1_MN
+                    Foundation : JavaScript
+                    Yes
+                    1
+                    4-7 years
+						</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -115,6 +136,10 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="3">
@@ -332,6 +357,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -657,8 +686,8 @@
   <dimension ref="A1:I933"/>
   <sheetViews>
     <sheetView topLeftCell="G1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A905" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:I933"/>
+      <pane ySplit="1" topLeftCell="A914" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I925" sqref="I925"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10076,7 +10105,7 @@
   <dimension ref="A1:F933"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10108,7 +10137,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="58.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>18</v>
       </c>
@@ -10124,11 +10153,11 @@
       <c r="E2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F2" t="s">
-        <v>13</v>
+      <c r="F2" s="3" t="s">
+        <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>18</v>
       </c>
@@ -10144,8 +10173,8 @@
       <c r="E3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F3" t="s">
-        <v>17</v>
+      <c r="F3" s="3" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -10161,6 +10190,9 @@
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
+      <c r="F5" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
@@ -10168,6 +10200,9 @@
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
+      <c r="F6" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
@@ -10239,112 +10274,115 @@
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F31" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -16659,6 +16697,7 @@
       <c r="E933" s="3"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>

<commit_message>
progress bar added asynchronously
</commit_message>
<xml_diff>
--- a/Active 20260120 - Copy.xlsx
+++ b/Active 20260120 - Copy.xlsx
@@ -5,16 +5,17 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c5e77caf6b479126/Documents/Beeline JD Parser/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\OneDrive\Documents\Beeline JD Parser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="13_ncr:1_{49132ED0-984B-4905-BBD2-F197B89F9026}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5E475747-C7AD-4F86-8680-92EC3026CD3B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03B3127E-D709-4684-906D-CA6B7B3F0411}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Job Postings" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="24">
   <si>
     <t>Job Code</t>
   </si>
@@ -357,10 +358,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -686,8 +683,8 @@
   <dimension ref="A1:I933"/>
   <sheetViews>
     <sheetView topLeftCell="G1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A914" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I925" sqref="I925"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G1" sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10104,7 +10101,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AFA9290-0450-455A-A954-670CFB09B6B7}">
   <dimension ref="A1:F933"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
@@ -16703,4 +16700,81 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC3CDA76-AF1A-4B01-B379-9FFD052D2AEF}">
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="9" max="9" width="255.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="3" t="str">
+        <f>IF(Table1[[#This Row],[Job Modified On]]-Table1[[#This Row],[Job Created]]&gt;30,"Yes","")</f>
+        <v/>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>